<commit_message>
Added Tolerance and Rounding
</commit_message>
<xml_diff>
--- a/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
+++ b/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840"/>
   </bookViews>
   <sheets>
     <sheet name="Assert1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>object_id</t>
   </si>
@@ -49,16 +49,35 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Global Tolerance</t>
+  </si>
+  <si>
+    <t>RoundingStyle</t>
+  </si>
+  <si>
+    <t>RoundingStep</t>
+  </si>
+  <si>
+    <t>1.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000000"/>
+    <numFmt numFmtId="171" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,16 +93,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,19 +135,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
+    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,103 +505,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:P1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
-        <v>29221</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="5">
+        <v>29221</v>
+      </c>
+      <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>29221</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="D10" s="10">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="5">
+        <v>29221</v>
+      </c>
+      <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>29221</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="5">
+        <v>29221</v>
+      </c>
+      <c r="C12" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>29221</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="D12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="5">
+        <v>29221</v>
+      </c>
+      <c r="C13" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>29221</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="5">
+        <v>29221</v>
+      </c>
+      <c r="C14" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D14" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Identity Insert Option
</commit_message>
<xml_diff>
--- a/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
+++ b/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840"/>
   </bookViews>
   <sheets>
-    <sheet name="Assert1" sheetId="1" r:id="rId1"/>
+    <sheet name="dbo#Sandbox" sheetId="1" r:id="rId1"/>
     <sheet name="Assert2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>object_id</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>dbo</t>
+  </si>
+  <si>
+    <t>Sandbox</t>
+  </si>
+  <si>
+    <t>IdentityInsert</t>
+  </si>
+  <si>
+    <t>identitytest</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>01.01.1980</t>
+  </si>
+  <si>
+    <t>0691BAF4-42D5-4702-B8EE-947B25EA532A</t>
+  </si>
+  <si>
+    <t>guid</t>
   </si>
 </sst>
 </file>
@@ -505,41 +529,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -549,112 +577,181 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
-        <v>29221</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="10">
+      <c r="E10" s="3">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
-        <v>29221</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
-        <v>29221</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
         <v>6</v>
       </c>
-      <c r="D12" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
-        <v>29221</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
         <v>7</v>
       </c>
-      <c r="D13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="5">
-        <v>29221</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
         <v>8</v>
       </c>
-      <c r="D14" s="2">
-        <v>4</v>
-      </c>
+      <c r="E14" s="3">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="5"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="5"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed Global Tolerance / fixed Variable Replacement
</commit_message>
<xml_diff>
--- a/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
+++ b/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dbo#ExcelTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>object_id</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Tolerance</t>
-  </si>
-  <si>
-    <t>Global Tolerance</t>
   </si>
   <si>
     <t>RoundingStyle</t>
@@ -524,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,13 +540,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -557,25 +554,25 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6">
-        <v>5</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
@@ -589,144 +586,139 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
         <v>17</v>
-      </c>
-      <c r="D11" s="3">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" s="3">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3">
-        <v>4</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="4"/>
@@ -742,11 +734,6 @@
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="4"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -756,10 +743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,13 +761,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -788,25 +775,25 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6">
-        <v>5</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
@@ -820,138 +807,128 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
         <v>17</v>
-      </c>
-      <c r="D11" s="3">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" s="3">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" s="3">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3">
-        <v>4</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added StdOut to Runcommand
</commit_message>
<xml_diff>
--- a/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
+++ b/NBi.Testing/Acceptance/Resources/Excel/Sample.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18100" windowHeight="13840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dbo#ExcelTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Assert" sheetId="2" r:id="rId2"/>
+    <sheet name="dbo#ExcelTest2" sheetId="3" r:id="rId2"/>
+    <sheet name="dbo#ExcelTest3" sheetId="4" r:id="rId3"/>
+    <sheet name="Assert" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="21">
   <si>
     <t>object_id</t>
   </si>
@@ -85,6 +87,9 @@
   </si>
   <si>
     <t>5,5</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -523,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:J7"/>
     </sheetView>
   </sheetViews>
@@ -758,6 +763,482 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="4"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="4"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>

</xml_diff>